<commit_message>
Updated dependencies from most recent master branch
</commit_message>
<xml_diff>
--- a/dependencies/mycobacterium/tbc/af2122/script_dependents/DefiningSNPsGroupDesignations.xlsx
+++ b/dependencies/mycobacterium/tbc/af2122/script_dependents/DefiningSNPsGroupDesignations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="342">
   <si>
     <t>Mbovis-01</t>
   </si>
@@ -650,9 +650,6 @@
     <t>NC_002945.4-2108312</t>
   </si>
   <si>
-    <t>NC_002945.4-2134170</t>
-  </si>
-  <si>
     <t>NC_002945.4-2138896</t>
   </si>
   <si>
@@ -1038,6 +1035,21 @@
   </si>
   <si>
     <t>Mbovis-37</t>
+  </si>
+  <si>
+    <t>Mbovis-17H</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1336004</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1098017</t>
+  </si>
+  <si>
+    <t>Mbovis-23B3</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3149672</t>
   </si>
 </sst>
 </file>
@@ -2039,10 +2051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E169"/>
+  <dimension ref="A1:E171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="129" zoomScaleNormal="129" zoomScalePageLayoutView="129" workbookViewId="0">
-      <selection activeCell="A157" sqref="A157"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="129" zoomScaleNormal="129" zoomScalePageLayoutView="129" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2065,7 +2077,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2081,7 +2093,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2097,7 +2109,7 @@
         <v>37</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2105,7 +2117,7 @@
         <v>38</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2121,7 +2133,7 @@
         <v>40</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2129,7 +2141,7 @@
         <v>41</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2137,7 +2149,7 @@
         <v>42</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2145,7 +2157,7 @@
         <v>43</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2161,7 +2173,7 @@
         <v>45</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2169,7 +2181,7 @@
         <v>46</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2177,7 +2189,7 @@
         <v>47</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2201,7 +2213,7 @@
         <v>50</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2217,7 +2229,7 @@
         <v>52</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2225,7 +2237,7 @@
         <v>53</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2265,7 +2277,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2273,7 +2285,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2289,7 +2301,7 @@
         <v>58</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2297,7 +2309,7 @@
         <v>59</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2345,23 +2357,23 @@
         <v>65</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>327</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2377,7 +2389,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2385,7 +2397,7 @@
         <v>67</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2393,7 +2405,7 @@
         <v>68</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2401,7 +2413,7 @@
         <v>5</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2409,7 +2421,7 @@
         <v>69</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2425,7 +2437,7 @@
         <v>6</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2457,7 +2469,7 @@
         <v>74</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2486,10 +2498,10 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>333</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2497,7 +2509,7 @@
         <v>9</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2505,39 +2517,39 @@
         <v>10</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2558,23 +2570,23 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>144</v>
@@ -2582,7 +2594,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>185</v>
@@ -2590,18 +2602,18 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2609,7 +2621,7 @@
         <v>13</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2617,15 +2629,15 @@
         <v>76</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2633,12 +2645,12 @@
         <v>77</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>165</v>
@@ -2646,34 +2658,34 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>281</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>283</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2681,7 +2693,7 @@
         <v>14</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2713,7 +2725,7 @@
         <v>80</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -2753,7 +2765,7 @@
         <v>84</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -2761,7 +2773,7 @@
         <v>85</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2769,7 +2781,7 @@
         <v>86</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2801,7 +2813,7 @@
         <v>90</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2809,7 +2821,7 @@
         <v>91</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -2817,7 +2829,7 @@
         <v>92</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>208</v>
+        <v>339</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2825,7 +2837,7 @@
         <v>93</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -2846,570 +2858,586 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>17</v>
+        <v>337</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>158</v>
+        <v>338</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>255</v>
+        <v>174</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>181</v>
+        <v>261</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>221</v>
+        <v>181</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>187</v>
+        <v>220</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>244</v>
+        <v>192</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>20</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>102</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B112" s="3" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>103</v>
+      <c r="A117" s="1" t="s">
+        <v>292</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>190</v>
+        <v>295</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>317</v>
+        <v>103</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>319</v>
+        <v>190</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>316</v>
+      </c>
+      <c r="B119" s="3" t="s">
         <v>318</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>21</v>
+        <v>320</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>228</v>
+        <v>321</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>104</v>
+        <v>22</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>143</v>
+        <v>212</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>196</v>
+        <v>143</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>133</v>
+        <v>237</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>220</v>
+        <v>137</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>313</v>
+        <v>219</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>314</v>
+        <v>340</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>264</v>
+        <v>341</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>315</v>
+        <v>109</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>202</v>
+        <v>312</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>236</v>
+        <v>263</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>117</v>
+        <v>314</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>175</v>
+        <v>202</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>110</v>
+        <v>315</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>183</v>
+        <v>235</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>24</v>
+        <v>110</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>186</v>
+        <v>142</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>203</v>
+        <v>149</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>111</v>
+        <v>26</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>166</v>
+        <v>203</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>111</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>28</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>29</v>
       </c>
-      <c r="B142" s="3" t="s">
+      <c r="B144" s="3" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>242</v>
+        <v>215</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>132</v>
+        <v>264</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>206</v>
+        <v>241</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>246</v>
+        <v>132</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>167</v>
+        <v>206</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>195</v>
+        <v>245</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B151" s="3" t="s">
+      <c r="B153" s="3" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>30</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>31</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>114</v>
+        <v>31</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>219</v>
+        <v>240</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>337</v>
+        <v>114</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>336</v>
+        <v>218</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>33</v>
+        <v>115</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>252</v>
+        <v>173</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>122</v>
+        <v>336</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>136</v>
+        <v>335</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>118</v>
+        <v>33</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>163</v>
+        <v>251</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>256</v>
+        <v>163</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>120</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>121</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>328</v>
+      </c>
+      <c r="B166" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="B164" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166"/>
-      <c r="B166"/>
-      <c r="D166" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="E166" s="8" t="s">
-        <v>306</v>
-      </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167"/>
-      <c r="B167"/>
-      <c r="D167" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="E167" s="7" t="s">
-        <v>307</v>
+      <c r="A167" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168"/>
       <c r="B168"/>
       <c r="D168" s="6" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="E168" s="8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169"/>
       <c r="B169"/>
       <c r="D169" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="E169" s="7" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170"/>
+      <c r="B170"/>
+      <c r="D170" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E170" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171"/>
+      <c r="B171"/>
+      <c r="D171" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E171" s="7" t="s">
         <v>310</v>
-      </c>
-      <c r="E169" s="7" t="s">
-        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>